<commit_message>
Progreso al cargar las bases de datos y primer iteración de la calculadora
</commit_message>
<xml_diff>
--- a/Marplatenses.xlsx
+++ b/Marplatenses.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matia\Desktop\Matias\Calculadora Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F23ED9-D026-4A52-8C1B-30777B303B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D90CAE-92C9-4236-828B-72E6B99F89A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{17E719AD-E269-4503-B3EE-09DDC3D8DFAA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Margarina</t>
   </si>
@@ -69,22 +69,44 @@
   </si>
   <si>
     <t>Bicarbonato de Sodio</t>
+  </si>
+  <si>
+    <t>150g</t>
+  </si>
+  <si>
+    <t>50g</t>
+  </si>
+  <si>
+    <t>5g</t>
+  </si>
+  <si>
+    <t>2g</t>
+  </si>
+  <si>
+    <t>250g</t>
+  </si>
+  <si>
+    <t>20g</t>
+  </si>
+  <si>
+    <t>1 u</t>
+  </si>
+  <si>
+    <t>1/2 u</t>
+  </si>
+  <si>
+    <t>1 tsp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,9 +134,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,120 +454,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EB8183-E77D-4010-886B-DBEA1CD9DBF8}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA437EC-220A-4A05-9500-77546CE1BC4E}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
-        <v>0.05</v>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>2E-3</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B12">
-    <sortCondition ref="A1:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:L2">
+    <sortCondition ref="A1:L1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Carga inicial de datos y cálculo de costo listos, falta capacidad de manipular bases de datos luego de cargadas
</commit_message>
<xml_diff>
--- a/Marplatenses.xlsx
+++ b/Marplatenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matia\Desktop\Matias\Calculadora Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D90CAE-92C9-4236-828B-72E6B99F89A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312A3B9-504F-45FC-BBFB-08695D9A2F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{17E719AD-E269-4503-B3EE-09DDC3D8DFAA}"/>
   </bookViews>
@@ -92,10 +92,10 @@
     <t>1 u</t>
   </si>
   <si>
-    <t>1/2 u</t>
-  </si>
-  <si>
     <t>1 tsp</t>
+  </si>
+  <si>
+    <t>1/2u</t>
   </si>
 </sst>
 </file>
@@ -103,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -140,7 +140,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
@@ -538,7 +538,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>12</v>
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>14</v>

</xml_diff>